<commit_message>
my commit description - sample2
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripts\production\files\git_local\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37134CBE-F31B-44F0-8D03-64CCF1777F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VMware" sheetId="1" r:id="rId1"/>
     <sheet name="Network Device" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="137">
   <si>
     <t>Greylock Federal Credit Union - HQ @ 75 Kellogg</t>
   </si>
@@ -436,12 +442,15 @@
   <si>
     <t>Network Device(13)</t>
   </si>
+  <si>
+    <t>updated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -527,10 +536,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -545,6 +554,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -591,7 +608,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,9 +640,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -657,6 +692,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -832,60 +885,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
@@ -899,7 +957,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -931,7 +989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -963,7 +1021,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -995,7 +1053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1027,7 +1085,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1091,7 +1149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1123,7 +1181,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1155,7 +1213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1187,7 +1245,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1251,7 +1309,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1283,7 +1341,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1325,96 +1383,96 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>135</v>
       </c>
@@ -1437,7 +1495,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>125</v>
       </c>
@@ -1460,7 +1518,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1519,7 +1577,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1578,7 +1636,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1637,7 +1695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1696,7 +1754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1755,7 +1813,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1814,7 +1872,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1873,7 +1931,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1932,7 +1990,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -1991,7 +2049,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -2050,7 +2108,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -2109,7 +2167,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2159,7 +2217,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>

</xml_diff>